<commit_message>
Update work_types excel file
</commit_message>
<xml_diff>
--- a/src/definitions/worktypes/work_types.xlsx
+++ b/src/definitions/worktypes/work_types.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\GitHub\crisiscleanup-web\src\definitions\worktypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB9A997-9DC0-4B7C-85BF-7DE82C69FA6E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726ECF60-6247-45B1-89F1-6A5BD0589C64}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1581,7 +1581,7 @@
   <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>